<commit_message>
Add a file logger for spread backtesting
</commit_message>
<xml_diff>
--- a/tools/scenarios_matrix.xlsx
+++ b/tools/scenarios_matrix.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
   <si>
     <t>initial_date</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -64,10 +64,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>210210.IB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>基准日</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -136,19 +132,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>200009.IB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>200202.IB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>220206.IB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>229914.IB</t>
+    <t>092218001.IB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>180210.IB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>200205.IB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>220220.IB</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -538,7 +534,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -549,66 +545,66 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.75" customWidth="1"/>
+    <col min="1" max="1" width="17.25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="99.625" customWidth="1"/>
     <col min="3" max="3" width="70.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="6">
-        <v>44739</v>
+        <v>45013</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="5">
         <v>0.02</v>
@@ -619,10 +615,10 @@
         <v>8</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -630,10 +626,10 @@
         <v>7</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -641,10 +637,10 @@
         <v>0</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -652,10 +648,10 @@
         <v>1</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -663,10 +659,10 @@
         <v>2</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -674,10 +670,10 @@
         <v>3</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -685,10 +681,10 @@
         <v>4</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -696,10 +692,10 @@
         <v>5</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -707,10 +703,10 @@
         <v>6</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>16</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -721,10 +717,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -768,18 +764,18 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>13000</v>
       </c>
       <c r="C2" t="str">
         <f>IF(A2&lt;&gt;"",[1]!b_info_carrydate(A2),"")</f>
-        <v>2020-07-02</v>
+        <v>2022-02-21</v>
       </c>
       <c r="D2" t="str">
         <f>IF(A2&lt;&gt;"",[1]!b_info_maturitydate(A2),"")</f>
-        <v>2023-07-02</v>
+        <v>2024-02-21</v>
       </c>
       <c r="E2" s="3">
         <f>IF(A2&lt;&gt;"",[1]!b_issue_issueprice(A2),"")</f>
@@ -787,7 +783,7 @@
       </c>
       <c r="F2" s="3">
         <f>IF(A2&lt;&gt;"",[1]!b_info_couponrate(A2),"")</f>
-        <v>2.36</v>
+        <v>2.27</v>
       </c>
       <c r="G2" t="str">
         <f>IF(A2&lt;&gt;"",[1]!b_info_coupon(A2),"")</f>
@@ -799,23 +795,23 @@
       </c>
       <c r="I2" s="3">
         <f>IF(A2&lt;&gt;"",[1]!b_anal_yield_cnbd(A2,parameter!C$2,1),"")</f>
-        <v>2.0449999999999999</v>
+        <v>2.4525000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>11000</v>
       </c>
       <c r="C3" t="str">
         <f>IF(A3&lt;&gt;"",[1]!b_info_carrydate(A3),"")</f>
-        <v>2020-04-09</v>
+        <v>2018-07-06</v>
       </c>
       <c r="D3" t="str">
         <f>IF(A3&lt;&gt;"",[1]!b_info_maturitydate(A3),"")</f>
-        <v>2023-04-09</v>
+        <v>2028-07-06</v>
       </c>
       <c r="E3" s="3">
         <f>IF(A3&lt;&gt;"",[1]!b_issue_issueprice(A3),"")</f>
@@ -823,7 +819,7 @@
       </c>
       <c r="F3" s="3">
         <f>IF(A3&lt;&gt;"",[1]!b_info_couponrate(A3),"")</f>
-        <v>1.86</v>
+        <v>4.04</v>
       </c>
       <c r="G3" t="str">
         <f>IF(A3&lt;&gt;"",[1]!b_info_coupon(A3),"")</f>
@@ -835,23 +831,23 @@
       </c>
       <c r="I3" s="3">
         <f>IF(A3&lt;&gt;"",[1]!b_anal_yield_cnbd(A3,parameter!C$2,1),"")</f>
-        <v>2.0352999999999999</v>
+        <v>2.9049999999999998</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>7000</v>
       </c>
       <c r="C4" t="str">
         <f>IF(A4&lt;&gt;"",[1]!b_info_carrydate(A4),"")</f>
-        <v>2021-06-07</v>
+        <v>2020-03-10</v>
       </c>
       <c r="D4" t="str">
         <f>IF(A4&lt;&gt;"",[1]!b_info_maturitydate(A4),"")</f>
-        <v>2031-06-07</v>
+        <v>2030-03-10</v>
       </c>
       <c r="E4" s="3">
         <f>IF(A4&lt;&gt;"",[1]!b_issue_issueprice(A4),"")</f>
@@ -859,7 +855,7 @@
       </c>
       <c r="F4" s="3">
         <f>IF(A4&lt;&gt;"",[1]!b_info_couponrate(A4),"")</f>
-        <v>3.41</v>
+        <v>3.07</v>
       </c>
       <c r="G4" t="str">
         <f>IF(A4&lt;&gt;"",[1]!b_info_coupon(A4),"")</f>
@@ -871,7 +867,7 @@
       </c>
       <c r="I4" s="3">
         <f>IF(A4&lt;&gt;"",[1]!b_anal_yield_cnbd(A4,parameter!C$2,1),"")</f>
-        <v>3.1524999999999999</v>
+        <v>3.0049999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -879,15 +875,15 @@
         <v>29</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>19000</v>
       </c>
       <c r="C5" t="str">
         <f>IF(A5&lt;&gt;"",[1]!b_info_carrydate(A5),"")</f>
-        <v>2022-05-23</v>
+        <v>2022-10-24</v>
       </c>
       <c r="D5" t="str">
         <f>IF(A5&lt;&gt;"",[1]!b_info_maturitydate(A5),"")</f>
-        <v>2023-05-23</v>
+        <v>2032-10-24</v>
       </c>
       <c r="E5" s="3">
         <f>IF(A5&lt;&gt;"",[1]!b_issue_issueprice(A5),"")</f>
@@ -895,55 +891,19 @@
       </c>
       <c r="F5" s="3">
         <f>IF(A5&lt;&gt;"",[1]!b_info_couponrate(A5),"")</f>
-        <v>1.83</v>
+        <v>2.77</v>
       </c>
       <c r="G5" t="str">
         <f>IF(A5&lt;&gt;"",[1]!b_info_coupon(A5),"")</f>
-        <v>到期一次还本付息</v>
+        <v>附息</v>
       </c>
       <c r="H5">
         <f>IF(A5&lt;&gt;"",[1]!b_info_interestfrequency(A5),"")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" s="3">
         <f>IF(A5&lt;&gt;"",[1]!b_anal_yield_cnbd(A5,parameter!C$2,1),"")</f>
-        <v>2.0550000000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6">
-        <v>40000</v>
-      </c>
-      <c r="C6" t="str">
-        <f>IF(A6&lt;&gt;"",[1]!b_info_carrydate(A6),"")</f>
-        <v>2022-04-11</v>
-      </c>
-      <c r="D6" t="str">
-        <f>IF(A6&lt;&gt;"",[1]!b_info_maturitydate(A6),"")</f>
-        <v>2022-07-11</v>
-      </c>
-      <c r="E6" s="3">
-        <f>IF(A6&lt;&gt;"",[1]!b_issue_issueprice(A6),"")</f>
-        <v>99.570999999999998</v>
-      </c>
-      <c r="F6" s="3">
-        <f>IF(A6&lt;&gt;"",[1]!b_info_couponrate(A6),"")</f>
-        <v>1.7269000000000001</v>
-      </c>
-      <c r="G6" t="str">
-        <f>IF(A6&lt;&gt;"",[1]!b_info_coupon(A6),"")</f>
-        <v>贴现</v>
-      </c>
-      <c r="H6">
-        <f>IF(A6&lt;&gt;"",[1]!b_info_interestfrequency(A6),"")</f>
-        <v>0</v>
-      </c>
-      <c r="I6" s="3">
-        <f>IF(A6&lt;&gt;"",[1]!b_anal_yield_cnbd(A6,parameter!C$2,1),"")</f>
-        <v>1.5398000000000001</v>
+        <v>3.048</v>
       </c>
     </row>
   </sheetData>

</xml_diff>